<commit_message>
atualização da home e finalização do sistema de chat global
</commit_message>
<xml_diff>
--- a/backend/BD/users.xlsx
+++ b/backend/BD/users.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -458,9 +458,93 @@
         <v>adrianep34@gmail.com</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>ee6ad9eb-fec3-457e-9f42-80c74b5eb51d</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Daniel</v>
+      </c>
+      <c r="C5" t="str">
+        <v>1377</v>
+      </c>
+      <c r="D5" t="str">
+        <v>fmasadlkf@gmail.com</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>14b55562-9898-4b6d-8036-b64846824fae</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Enrique</v>
+      </c>
+      <c r="C6" t="str">
+        <v>2101</v>
+      </c>
+      <c r="D6" t="str">
+        <v>enrique@gmail.com</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>3102bfaf-f1d4-46f3-8745-c401a0151a78</v>
+      </c>
+      <c r="B7" t="str">
+        <v>fkdjasç</v>
+      </c>
+      <c r="C7" t="str">
+        <v>12</v>
+      </c>
+      <c r="D7" t="str">
+        <v>jfhalksdjh@gmail.com</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>3bfadc1d-7458-4960-bddd-28c6367c6473</v>
+      </c>
+      <c r="B8" t="str">
+        <v>dsafds</v>
+      </c>
+      <c r="C8" t="str">
+        <v>21</v>
+      </c>
+      <c r="D8" t="str">
+        <v>dfasdf@gmail.com</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>4b7488d0-fe4f-46cc-b519-e058bd2be3b7</v>
+      </c>
+      <c r="B9" t="str">
+        <v>sdadf</v>
+      </c>
+      <c r="C9" t="str">
+        <v>21</v>
+      </c>
+      <c r="D9" t="str">
+        <v>fasdfsdf@gmial.com</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>5ad53af3-4018-4fea-b2c4-00b6937ba621</v>
+      </c>
+      <c r="B10" t="str">
+        <v>murilo</v>
+      </c>
+      <c r="C10" t="str">
+        <v>murilo20</v>
+      </c>
+      <c r="D10" t="str">
+        <v>muriloluiz380@gmail.com</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>